<commit_message>
removes mauricio, deletes old files and transfer last optimization to old folder
</commit_message>
<xml_diff>
--- a/src/results/old/two_evaporators_cop.xlsx
+++ b/src/results/old/two_evaporators_cop.xlsx
@@ -1,26 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repositories\projeto-final\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repositories\projeto-final\src\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD962DB7-D397-4BA5-B64B-457E1AF2267D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB861890-6A95-4D35-879E-8EE40C0A5047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$109</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="38">
   <si>
     <t>refrigerant</t>
   </si>
@@ -115,16 +118,25 @@
     <t>R134a</t>
   </si>
   <si>
+    <t>R1234yf</t>
+  </si>
+  <si>
+    <t>R1234ze(E)</t>
+  </si>
+  <si>
     <t>R22</t>
   </si>
   <si>
     <t>R290</t>
   </si>
   <si>
-    <t>R1234yf</t>
+    <t>NH3</t>
   </si>
   <si>
-    <t>NH3</t>
+    <t>R404a</t>
+  </si>
+  <si>
+    <t>R410a</t>
   </si>
 </sst>
 </file>
@@ -487,29 +499,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q73"/>
+  <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1848,46 +1860,46 @@
         <v>18</v>
       </c>
       <c r="D26">
-        <v>63.888243018283802</v>
+        <v>68.570527268831</v>
       </c>
       <c r="E26">
-        <v>45.999534973164337</v>
+        <v>49.370779633558321</v>
       </c>
       <c r="F26">
-        <v>31.92367727137605</v>
+        <v>34.263321065689468</v>
       </c>
       <c r="G26">
-        <v>50.453771533682371</v>
+        <v>125.82115678227601</v>
       </c>
       <c r="H26">
-        <v>111.99670587608939</v>
+        <v>48.213205548500149</v>
       </c>
       <c r="I26">
         <v>10</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L26">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M26">
-        <v>0.51347246539093006</v>
+        <v>0.53205676622873577</v>
       </c>
       <c r="N26">
-        <v>2.5427288298299429</v>
+        <v>2.538034477239381</v>
       </c>
       <c r="O26">
-        <v>2.3478498220255082</v>
+        <v>2.187528752869647</v>
       </c>
       <c r="P26">
-        <v>0.39807550198506308</v>
+        <v>0.30433898054297098</v>
       </c>
       <c r="Q26">
-        <v>0.32771464537327261</v>
+        <v>0.30707401556350661</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -1901,46 +1913,46 @@
         <v>19</v>
       </c>
       <c r="D27">
-        <v>65.414191245523043</v>
+        <v>70.462746617623168</v>
       </c>
       <c r="E27">
-        <v>47.098217696776587</v>
+        <v>50.733177564688681</v>
       </c>
       <c r="F27">
-        <v>32.686163081562952</v>
+        <v>35.208825229893939</v>
       </c>
       <c r="G27">
-        <v>50.509024125002021</v>
+        <v>126.2200744429818</v>
       </c>
       <c r="H27">
-        <v>112.0781469938814</v>
+        <v>48.308399486127691</v>
       </c>
       <c r="I27">
         <v>10</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K27">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L27">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M27">
-        <v>0.51358398306536812</v>
+        <v>0.53248551770066987</v>
       </c>
       <c r="N27">
-        <v>2.485503038761653</v>
+        <v>2.4768900207114388</v>
       </c>
       <c r="O27">
-        <v>2.2930804026452898</v>
+        <v>2.128784459879173</v>
       </c>
       <c r="P27">
-        <v>0.39861865330577551</v>
+        <v>0.30615512238030201</v>
       </c>
       <c r="Q27">
-        <v>0.32872607153999112</v>
+        <v>0.30689648650116802</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -1954,46 +1966,46 @@
         <v>20</v>
       </c>
       <c r="D28">
-        <v>63.888243018283802</v>
+        <v>68.570527268831</v>
       </c>
       <c r="E28">
-        <v>45.999534973164337</v>
+        <v>49.370779633558321</v>
       </c>
       <c r="F28">
-        <v>31.92367727137605</v>
+        <v>34.263321065689468</v>
       </c>
       <c r="G28">
-        <v>50.453771533682371</v>
+        <v>125.82115678227601</v>
       </c>
       <c r="H28">
-        <v>111.99670587608939</v>
+        <v>48.213205548500149</v>
       </c>
       <c r="I28">
         <v>10</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L28">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M28">
-        <v>0.51347246539093006</v>
+        <v>0.53205676622873577</v>
       </c>
       <c r="N28">
-        <v>2.5427288298299429</v>
+        <v>2.538034477239381</v>
       </c>
       <c r="O28">
-        <v>2.3478498220255082</v>
+        <v>2.187528752869647</v>
       </c>
       <c r="P28">
-        <v>0.39807550198506308</v>
+        <v>0.30433898054297098</v>
       </c>
       <c r="Q28">
-        <v>0.32771464537327261</v>
+        <v>0.30707401556350661</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -2007,46 +2019,46 @@
         <v>21</v>
       </c>
       <c r="D29">
-        <v>62.384762842299097</v>
+        <v>66.723085809212307</v>
       </c>
       <c r="E29">
-        <v>44.917029246455357</v>
+        <v>48.040621782632861</v>
       </c>
       <c r="F29">
-        <v>31.172418297040011</v>
+        <v>33.340191517147197</v>
       </c>
       <c r="G29">
-        <v>50.399914254847523</v>
+        <v>125.4348126943699</v>
       </c>
       <c r="H29">
-        <v>111.9175690269544</v>
+        <v>48.121172361128643</v>
       </c>
       <c r="I29">
         <v>10</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L29">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M29">
-        <v>0.5133631778653317</v>
+        <v>0.53164060959584714</v>
       </c>
       <c r="N29">
-        <v>2.6018770591806248</v>
+        <v>2.60113846580423</v>
       </c>
       <c r="O29">
-        <v>2.4044332809147848</v>
+        <v>2.2480974640308049</v>
       </c>
       <c r="P29">
-        <v>0.39738812074090668</v>
+        <v>0.30229789983092459</v>
       </c>
       <c r="Q29">
-        <v>0.32653628928737721</v>
+        <v>0.30705671214913499</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -2060,46 +2072,46 @@
         <v>22</v>
       </c>
       <c r="D30">
-        <v>59.442271628607038</v>
+        <v>63.154436558463011</v>
       </c>
       <c r="E30">
-        <v>42.798435572597057</v>
+        <v>45.471194322093368</v>
       </c>
       <c r="F30">
-        <v>29.702114287382361</v>
+        <v>31.55700885953279</v>
       </c>
       <c r="G30">
-        <v>50.296166526600288</v>
+        <v>124.69743125362081</v>
       </c>
       <c r="H30">
-        <v>111.7658197722923</v>
+        <v>47.945948185147991</v>
       </c>
       <c r="I30">
         <v>10</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L30">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M30">
-        <v>0.51315100538703506</v>
+        <v>0.53084387124872967</v>
       </c>
       <c r="N30">
-        <v>2.7263760596406801</v>
+        <v>2.7336698551486589</v>
       </c>
       <c r="O30">
-        <v>2.5234567234777652</v>
+        <v>2.3751300490368989</v>
       </c>
       <c r="P30">
-        <v>0.3955555682029136</v>
+        <v>0.29750232122338222</v>
       </c>
       <c r="Q30">
-        <v>0.32364979831693519</v>
+        <v>0.30640925482616688</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -2113,46 +2125,46 @@
         <v>23</v>
       </c>
       <c r="D31">
-        <v>58.001875554335442</v>
+        <v>61.429479151733332</v>
       </c>
       <c r="E31">
-        <v>41.761350399121518</v>
+        <v>44.229224989248003</v>
       </c>
       <c r="F31">
-        <v>28.98237717699033</v>
+        <v>30.695082142538109</v>
       </c>
       <c r="G31">
-        <v>50.246174013910817</v>
+        <v>124.3452849054958</v>
       </c>
       <c r="H31">
-        <v>111.69302716806369</v>
+        <v>47.862464338082169</v>
       </c>
       <c r="I31">
         <v>10</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L31">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M31">
-        <v>0.51304798467728085</v>
+        <v>0.53046226682753017</v>
       </c>
       <c r="N31">
-        <v>2.7919649086221678</v>
+        <v>2.8033405397792448</v>
       </c>
       <c r="O31">
-        <v>2.58612326871192</v>
+        <v>2.4418243825491972</v>
       </c>
       <c r="P31">
-        <v>0.3943965753402694</v>
+        <v>0.29472660246458282</v>
       </c>
       <c r="Q31">
-        <v>0.32192566964963731</v>
+        <v>0.30576337948295929</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
@@ -2166,46 +2178,46 @@
         <v>24</v>
       </c>
       <c r="D32">
-        <v>56.581173663985822</v>
+        <v>59.741782206948571</v>
       </c>
       <c r="E32">
-        <v>40.738445038069777</v>
+        <v>43.014083189002967</v>
       </c>
       <c r="F32">
-        <v>28.27248085642043</v>
+        <v>29.851773733168059</v>
       </c>
       <c r="G32">
-        <v>50.197372283392603</v>
+        <v>124.0034877936392</v>
       </c>
       <c r="H32">
-        <v>111.6221776587754</v>
+        <v>47.781553711995578</v>
       </c>
       <c r="I32">
         <v>10</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L32">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M32">
-        <v>0.51294692221474292</v>
+        <v>0.53009120687357958</v>
       </c>
       <c r="N32">
-        <v>2.8599539292548628</v>
+        <v>2.8754589361020839</v>
       </c>
       <c r="O32">
-        <v>2.6510584755769342</v>
+        <v>2.5108055779185219</v>
       </c>
       <c r="P32">
-        <v>0.39306561310590821</v>
+        <v>0.29168335760040942</v>
       </c>
       <c r="Q32">
-        <v>0.3200025122659077</v>
+        <v>0.30489111892611392</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
@@ -2219,46 +2231,46 @@
         <v>25</v>
       </c>
       <c r="D33">
-        <v>58.001875554335442</v>
+        <v>61.429479151733332</v>
       </c>
       <c r="E33">
-        <v>41.761350399121518</v>
+        <v>44.229224989248003</v>
       </c>
       <c r="F33">
-        <v>28.98237717699033</v>
+        <v>30.695082142538109</v>
       </c>
       <c r="G33">
-        <v>50.246174013910817</v>
+        <v>124.3452849054958</v>
       </c>
       <c r="H33">
-        <v>111.69302716806369</v>
+        <v>47.862464338082169</v>
       </c>
       <c r="I33">
         <v>10</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L33">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M33">
-        <v>0.51304798467728085</v>
+        <v>0.53046226682753017</v>
       </c>
       <c r="N33">
-        <v>2.7919649086221678</v>
+        <v>2.8033405397792448</v>
       </c>
       <c r="O33">
-        <v>2.58612326871192</v>
+        <v>2.4418243825491972</v>
       </c>
       <c r="P33">
-        <v>0.3943965753402694</v>
+        <v>0.29472660246458282</v>
       </c>
       <c r="Q33">
-        <v>0.32192566964963731</v>
+        <v>0.30576337948295929</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
@@ -2272,46 +2284,46 @@
         <v>26</v>
       </c>
       <c r="D34">
-        <v>58.001875554335442</v>
+        <v>61.429479151733332</v>
       </c>
       <c r="E34">
-        <v>41.761350399121518</v>
+        <v>44.229224989248003</v>
       </c>
       <c r="F34">
-        <v>28.98237717699033</v>
+        <v>30.695082142538109</v>
       </c>
       <c r="G34">
-        <v>50.246174013910817</v>
+        <v>124.3452849054958</v>
       </c>
       <c r="H34">
-        <v>111.69302716806369</v>
+        <v>47.862464338082169</v>
       </c>
       <c r="I34">
         <v>10</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K34">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L34">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M34">
-        <v>0.51304798467728085</v>
+        <v>0.53046226682753017</v>
       </c>
       <c r="N34">
-        <v>2.7919649086221678</v>
+        <v>2.8033405397792448</v>
       </c>
       <c r="O34">
-        <v>2.58612326871192</v>
+        <v>2.4418243825491972</v>
       </c>
       <c r="P34">
-        <v>0.3943965753402694</v>
+        <v>0.29472660246458282</v>
       </c>
       <c r="Q34">
-        <v>0.32192566964963731</v>
+        <v>0.30576337948295929</v>
       </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
@@ -2325,46 +2337,46 @@
         <v>27</v>
       </c>
       <c r="D35">
-        <v>59.442271628607038</v>
+        <v>63.154436558463011</v>
       </c>
       <c r="E35">
-        <v>42.798435572597057</v>
+        <v>45.471194322093368</v>
       </c>
       <c r="F35">
-        <v>29.702114287382361</v>
+        <v>31.55700885953279</v>
       </c>
       <c r="G35">
-        <v>50.296166526600288</v>
+        <v>124.69743125362081</v>
       </c>
       <c r="H35">
-        <v>111.7658197722923</v>
+        <v>47.945948185147991</v>
       </c>
       <c r="I35">
         <v>10</v>
       </c>
       <c r="J35">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K35">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L35">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M35">
-        <v>0.51315100538703506</v>
+        <v>0.53084387124872967</v>
       </c>
       <c r="N35">
-        <v>2.7263760596406801</v>
+        <v>2.7336698551486589</v>
       </c>
       <c r="O35">
-        <v>2.5234567234777652</v>
+        <v>2.3751300490368989</v>
       </c>
       <c r="P35">
-        <v>0.3955555682029136</v>
+        <v>0.29750232122338222</v>
       </c>
       <c r="Q35">
-        <v>0.32364979831693519</v>
+        <v>0.30640925482616688</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.25">
@@ -2378,46 +2390,46 @@
         <v>28</v>
       </c>
       <c r="D36">
-        <v>60.903008519827928</v>
+        <v>64.918366246852145</v>
       </c>
       <c r="E36">
-        <v>43.850166134276108</v>
+        <v>46.741223697733538</v>
       </c>
       <c r="F36">
-        <v>30.432015297187611</v>
+        <v>32.438409246227067</v>
       </c>
       <c r="G36">
-        <v>50.347396741392451</v>
+        <v>125.0604285515934</v>
       </c>
       <c r="H36">
-        <v>111.84063791718761</v>
+        <v>48.032137099440767</v>
       </c>
       <c r="I36">
         <v>10</v>
       </c>
       <c r="J36">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K36">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L36">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M36">
-        <v>0.51325604768208211</v>
+        <v>0.53123648693348835</v>
       </c>
       <c r="N36">
-        <v>2.6630545616769861</v>
+        <v>2.6663111790714131</v>
       </c>
       <c r="O36">
-        <v>2.4629325159062572</v>
+        <v>2.3105941919367599</v>
       </c>
       <c r="P36">
-        <v>0.39655035709514957</v>
+        <v>0.30002241528958712</v>
       </c>
       <c r="Q36">
-        <v>0.32518390069663528</v>
+        <v>0.30683763730518587</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
@@ -2431,46 +2443,46 @@
         <v>29</v>
       </c>
       <c r="D37">
-        <v>62.384762842299097</v>
+        <v>66.723085809212307</v>
       </c>
       <c r="E37">
-        <v>44.917029246455357</v>
+        <v>48.040621782632861</v>
       </c>
       <c r="F37">
-        <v>31.172418297040011</v>
+        <v>33.340191517147197</v>
       </c>
       <c r="G37">
-        <v>50.399914254847523</v>
+        <v>125.4348126943699</v>
       </c>
       <c r="H37">
-        <v>111.9175690269544</v>
+        <v>48.121172361128643</v>
       </c>
       <c r="I37">
         <v>10</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K37">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L37">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M37">
-        <v>0.5133631778653317</v>
+        <v>0.53164060959584714</v>
       </c>
       <c r="N37">
-        <v>2.6018770591806248</v>
+        <v>2.60113846580423</v>
       </c>
       <c r="O37">
-        <v>2.4044332809147848</v>
+        <v>2.2480974640308049</v>
       </c>
       <c r="P37">
-        <v>0.39738812074090668</v>
+        <v>0.30229789983092459</v>
       </c>
       <c r="Q37">
-        <v>0.32653628928737721</v>
+        <v>0.30705671214913499</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
@@ -2484,19 +2496,19 @@
         <v>18</v>
       </c>
       <c r="D38">
-        <v>65.417649009978234</v>
+        <v>65.319804929048559</v>
       </c>
       <c r="E38">
-        <v>47.100707287184328</v>
+        <v>47.030259548914962</v>
       </c>
       <c r="F38">
-        <v>32.687890857305931</v>
+        <v>32.639000126946982</v>
       </c>
       <c r="G38">
-        <v>119.4188407022428</v>
+        <v>122.0311691531135</v>
       </c>
       <c r="H38">
-        <v>47.181613456933277</v>
+        <v>47.273690685173563</v>
       </c>
       <c r="I38">
         <v>10</v>
@@ -2511,19 +2523,19 @@
         <v>0.3</v>
       </c>
       <c r="M38">
-        <v>0.52219352782079764</v>
+        <v>0.52854418540590031</v>
       </c>
       <c r="N38">
-        <v>2.546720291549522</v>
+        <v>2.5919376217088939</v>
       </c>
       <c r="O38">
-        <v>2.2929591978629551</v>
+        <v>2.2963938756849078</v>
       </c>
       <c r="P38">
-        <v>0.3061446329919425</v>
+        <v>0.31121916490760532</v>
       </c>
       <c r="Q38">
-        <v>0.32089401057272721</v>
+        <v>0.32222953780250829</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
@@ -2537,19 +2549,19 @@
         <v>19</v>
       </c>
       <c r="D39">
-        <v>67.078556952777859</v>
+        <v>66.990771344403072</v>
       </c>
       <c r="E39">
-        <v>48.296561006000061</v>
+        <v>48.233355367970212</v>
       </c>
       <c r="F39">
-        <v>33.517813338164054</v>
+        <v>33.473948625371328</v>
       </c>
       <c r="G39">
-        <v>119.67472060686011</v>
+        <v>122.3076770714205</v>
       </c>
       <c r="H39">
-        <v>47.249326341937604</v>
+        <v>47.336611946514672</v>
       </c>
       <c r="I39">
         <v>10</v>
@@ -2564,19 +2576,19 @@
         <v>0.3</v>
       </c>
       <c r="M39">
-        <v>0.52242760720006809</v>
+        <v>0.52886191116729364</v>
       </c>
       <c r="N39">
-        <v>2.4884859563438329</v>
+        <v>2.5323531228769558</v>
       </c>
       <c r="O39">
-        <v>2.236184062599877</v>
+        <v>2.239114388291517</v>
       </c>
       <c r="P39">
-        <v>0.30834980686732699</v>
+        <v>0.31342702237246528</v>
       </c>
       <c r="Q39">
-        <v>0.32140333230003237</v>
+        <v>0.32267113562321342</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
@@ -2590,19 +2602,19 @@
         <v>20</v>
       </c>
       <c r="D40">
-        <v>65.417649009978234</v>
+        <v>65.319804929048559</v>
       </c>
       <c r="E40">
-        <v>47.100707287184328</v>
+        <v>47.030259548914962</v>
       </c>
       <c r="F40">
-        <v>32.687890857305931</v>
+        <v>32.639000126946982</v>
       </c>
       <c r="G40">
-        <v>119.4188407022428</v>
+        <v>122.0311691531135</v>
       </c>
       <c r="H40">
-        <v>47.181613456933277</v>
+        <v>47.273690685173563</v>
       </c>
       <c r="I40">
         <v>10</v>
@@ -2617,19 +2629,19 @@
         <v>0.3</v>
       </c>
       <c r="M40">
-        <v>0.52219352782079764</v>
+        <v>0.52854418540590031</v>
       </c>
       <c r="N40">
-        <v>2.546720291549522</v>
+        <v>2.5919376217088939</v>
       </c>
       <c r="O40">
-        <v>2.2929591978629551</v>
+        <v>2.2963938756849078</v>
       </c>
       <c r="P40">
-        <v>0.3061446329919425</v>
+        <v>0.31121916490760532</v>
       </c>
       <c r="Q40">
-        <v>0.32089401057272721</v>
+        <v>0.32222953780250829</v>
       </c>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
@@ -2643,19 +2655,19 @@
         <v>21</v>
       </c>
       <c r="D41">
-        <v>63.787840732247993</v>
+        <v>63.680393745258478</v>
       </c>
       <c r="E41">
-        <v>45.92724532721855</v>
+        <v>45.849883496586102</v>
       </c>
       <c r="F41">
-        <v>31.873508257089679</v>
+        <v>31.819819146630749</v>
       </c>
       <c r="G41">
-        <v>119.16996704243761</v>
+        <v>121.7619276724941</v>
       </c>
       <c r="H41">
-        <v>47.115867699615677</v>
+        <v>47.212533570955578</v>
       </c>
       <c r="I41">
         <v>10</v>
@@ -2670,19 +2682,19 @@
         <v>0.3</v>
       </c>
       <c r="M41">
-        <v>0.52196523933676098</v>
+        <v>0.52823418393276567</v>
       </c>
       <c r="N41">
-        <v>2.6068578718637729</v>
+        <v>2.6534770171082869</v>
       </c>
       <c r="O41">
-        <v>2.351545345916803</v>
+        <v>2.3555130736164571</v>
       </c>
       <c r="P41">
-        <v>0.30372978986510951</v>
+        <v>0.308797536917649</v>
       </c>
       <c r="Q41">
-        <v>0.32020255991575147</v>
+        <v>0.3216062366606578</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
@@ -2696,19 +2708,19 @@
         <v>22</v>
       </c>
       <c r="D42">
-        <v>60.616656149042228</v>
+        <v>60.491424296583183</v>
       </c>
       <c r="E42">
-        <v>43.643992427310401</v>
+        <v>43.553825493539897</v>
       </c>
       <c r="F42">
-        <v>30.288930744553419</v>
+        <v>30.226354892516682</v>
       </c>
       <c r="G42">
-        <v>118.69205806099301</v>
+        <v>121.244096366284</v>
       </c>
       <c r="H42">
-        <v>46.9899295195438</v>
+        <v>47.095220347616397</v>
       </c>
       <c r="I42">
         <v>10</v>
@@ -2723,19 +2735,19 @@
         <v>0.3</v>
       </c>
       <c r="M42">
-        <v>0.52152515692786794</v>
+        <v>0.52763621526758342</v>
       </c>
       <c r="N42">
-        <v>2.7332749462979842</v>
+        <v>2.7828625077258922</v>
       </c>
       <c r="O42">
-        <v>2.474567380146885</v>
+        <v>2.4796903320471602</v>
       </c>
       <c r="P42">
-        <v>0.29823367213557822</v>
+        <v>0.30327429578628151</v>
       </c>
       <c r="Q42">
-        <v>0.31824478662720979</v>
+        <v>0.31978520366492208</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
@@ -2749,19 +2761,19 @@
         <v>23</v>
       </c>
       <c r="D43">
-        <v>59.073001990560023</v>
+        <v>58.939607772334973</v>
       </c>
       <c r="E43">
-        <v>42.532561433203213</v>
+        <v>42.436517596081167</v>
       </c>
       <c r="F43">
-        <v>29.517597634643032</v>
+        <v>29.450943211680329</v>
       </c>
       <c r="G43">
-        <v>118.4624734194721</v>
+        <v>120.99496954286801</v>
       </c>
       <c r="H43">
-        <v>46.929575505113263</v>
+        <v>47.038928102994781</v>
       </c>
       <c r="I43">
         <v>10</v>
@@ -2776,19 +2788,19 @@
         <v>0.3</v>
       </c>
       <c r="M43">
-        <v>0.52131295209185735</v>
+        <v>0.52734771369118516</v>
       </c>
       <c r="N43">
-        <v>2.7997908240894098</v>
+        <v>2.8509503879789029</v>
       </c>
       <c r="O43">
-        <v>2.539231035253132</v>
+        <v>2.5449779133142938</v>
       </c>
       <c r="P43">
-        <v>0.2951318234086634</v>
+        <v>0.30015144250045428</v>
       </c>
       <c r="Q43">
-        <v>0.31696271150964378</v>
+        <v>0.31857130582661292</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
@@ -2802,19 +2814,19 @@
         <v>24</v>
       </c>
       <c r="D44">
-        <v>57.555883754216318</v>
+        <v>57.414822657575577</v>
       </c>
       <c r="E44">
-        <v>41.440236303035753</v>
+        <v>41.338672313454417</v>
       </c>
       <c r="F44">
-        <v>28.759523994306811</v>
+        <v>28.689038585537361</v>
       </c>
       <c r="G44">
-        <v>118.238794121193</v>
+        <v>120.7520332425046</v>
       </c>
       <c r="H44">
-        <v>46.870864730574567</v>
+        <v>46.98412721900084</v>
       </c>
       <c r="I44">
         <v>10</v>
@@ -2829,19 +2841,19 @@
         <v>0.3</v>
       </c>
       <c r="M44">
-        <v>0.52110571487161983</v>
+        <v>0.52706586592669769</v>
       </c>
       <c r="N44">
-        <v>2.8686842783414348</v>
+        <v>2.921478334295152</v>
       </c>
       <c r="O44">
-        <v>2.6061627450731581</v>
+        <v>2.612565763628782</v>
       </c>
       <c r="P44">
-        <v>0.29177901560962272</v>
+        <v>0.29677219313995851</v>
       </c>
       <c r="Q44">
-        <v>0.31546689122119281</v>
+        <v>0.31714325969352197</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
@@ -2855,19 +2867,19 @@
         <v>25</v>
       </c>
       <c r="D45">
-        <v>59.073001990560023</v>
+        <v>58.939607772334973</v>
       </c>
       <c r="E45">
-        <v>42.532561433203213</v>
+        <v>42.436517596081167</v>
       </c>
       <c r="F45">
-        <v>29.517597634643032</v>
+        <v>29.450943211680329</v>
       </c>
       <c r="G45">
-        <v>118.4624734194721</v>
+        <v>120.99496954286801</v>
       </c>
       <c r="H45">
-        <v>46.929575505113263</v>
+        <v>47.038928102994781</v>
       </c>
       <c r="I45">
         <v>10</v>
@@ -2882,19 +2894,19 @@
         <v>0.3</v>
       </c>
       <c r="M45">
-        <v>0.52131295209185735</v>
+        <v>0.52734771369118516</v>
       </c>
       <c r="N45">
-        <v>2.7997908240894098</v>
+        <v>2.8509503879789029</v>
       </c>
       <c r="O45">
-        <v>2.539231035253132</v>
+        <v>2.5449779133142938</v>
       </c>
       <c r="P45">
-        <v>0.2951318234086634</v>
+        <v>0.30015144250045428</v>
       </c>
       <c r="Q45">
-        <v>0.31696271150964378</v>
+        <v>0.31857130582661292</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
@@ -2908,19 +2920,19 @@
         <v>26</v>
       </c>
       <c r="D46">
-        <v>59.073001990560023</v>
+        <v>58.939607772334973</v>
       </c>
       <c r="E46">
-        <v>42.532561433203213</v>
+        <v>42.436517596081167</v>
       </c>
       <c r="F46">
-        <v>29.517597634643032</v>
+        <v>29.450943211680329</v>
       </c>
       <c r="G46">
-        <v>118.4624734194721</v>
+        <v>120.99496954286801</v>
       </c>
       <c r="H46">
-        <v>46.929575505113263</v>
+        <v>47.038928102994781</v>
       </c>
       <c r="I46">
         <v>10</v>
@@ -2935,19 +2947,19 @@
         <v>0.3</v>
       </c>
       <c r="M46">
-        <v>0.52131295209185735</v>
+        <v>0.52734771369118516</v>
       </c>
       <c r="N46">
-        <v>2.7997908240894098</v>
+        <v>2.8509503879789029</v>
       </c>
       <c r="O46">
-        <v>2.539231035253132</v>
+        <v>2.5449779133142938</v>
       </c>
       <c r="P46">
-        <v>0.2951318234086634</v>
+        <v>0.30015144250045428</v>
       </c>
       <c r="Q46">
-        <v>0.31696271150964378</v>
+        <v>0.31857130582661292</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -2961,19 +2973,19 @@
         <v>27</v>
       </c>
       <c r="D47">
-        <v>60.616656149042228</v>
+        <v>60.491424296583183</v>
       </c>
       <c r="E47">
-        <v>43.643992427310401</v>
+        <v>43.553825493539897</v>
       </c>
       <c r="F47">
-        <v>30.288930744553419</v>
+        <v>30.226354892516682</v>
       </c>
       <c r="G47">
-        <v>118.69205806099301</v>
+        <v>121.244096366284</v>
       </c>
       <c r="H47">
-        <v>46.9899295195438</v>
+        <v>47.095220347616397</v>
       </c>
       <c r="I47">
         <v>10</v>
@@ -2988,19 +3000,19 @@
         <v>0.3</v>
       </c>
       <c r="M47">
-        <v>0.52152515692786794</v>
+        <v>0.52763621526758342</v>
       </c>
       <c r="N47">
-        <v>2.7332749462979842</v>
+        <v>2.7828625077258922</v>
       </c>
       <c r="O47">
-        <v>2.474567380146885</v>
+        <v>2.4796903320471602</v>
       </c>
       <c r="P47">
-        <v>0.29823367213557822</v>
+        <v>0.30327429578628151</v>
       </c>
       <c r="Q47">
-        <v>0.31824478662720979</v>
+        <v>0.31978520366492208</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
@@ -3014,19 +3026,19 @@
         <v>28</v>
       </c>
       <c r="D48">
-        <v>62.187899379591968</v>
+        <v>62.071319406848517</v>
       </c>
       <c r="E48">
-        <v>44.775287553306221</v>
+        <v>44.691349972930936</v>
       </c>
       <c r="F48">
-        <v>31.07404956199451</v>
+        <v>31.015796881214069</v>
       </c>
       <c r="G48">
-        <v>118.92780032253449</v>
+        <v>121.4996619321205</v>
       </c>
       <c r="H48">
-        <v>47.052000777818073</v>
+        <v>47.153066759697779</v>
       </c>
       <c r="I48">
         <v>10</v>
@@ -3041,19 +3053,19 @@
         <v>0.3</v>
       </c>
       <c r="M48">
-        <v>0.52174251932526505</v>
+        <v>0.52793161852252857</v>
       </c>
       <c r="N48">
-        <v>2.6690047864009649</v>
+        <v>2.7170798092171751</v>
       </c>
       <c r="O48">
-        <v>2.4120448109109969</v>
+        <v>2.4165750210144572</v>
       </c>
       <c r="P48">
-        <v>0.30109610109210211</v>
+        <v>0.30615265347797832</v>
       </c>
       <c r="Q48">
-        <v>0.31932200476969269</v>
+        <v>0.32079404723318589</v>
       </c>
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
@@ -3067,19 +3079,19 @@
         <v>29</v>
       </c>
       <c r="D49">
-        <v>63.787840732247993</v>
+        <v>63.680393745258478</v>
       </c>
       <c r="E49">
-        <v>45.92724532721855</v>
+        <v>45.849883496586102</v>
       </c>
       <c r="F49">
-        <v>31.873508257089679</v>
+        <v>31.819819146630749</v>
       </c>
       <c r="G49">
-        <v>119.16996704243761</v>
+        <v>121.7619276724941</v>
       </c>
       <c r="H49">
-        <v>47.115867699615677</v>
+        <v>47.212533570955578</v>
       </c>
       <c r="I49">
         <v>10</v>
@@ -3094,19 +3106,19 @@
         <v>0.3</v>
       </c>
       <c r="M49">
-        <v>0.52196523933676098</v>
+        <v>0.52823418393276567</v>
       </c>
       <c r="N49">
-        <v>2.6068578718637729</v>
+        <v>2.6534770171082869</v>
       </c>
       <c r="O49">
-        <v>2.351545345916803</v>
+        <v>2.3555130736164571</v>
       </c>
       <c r="P49">
-        <v>0.30372978986510951</v>
+        <v>0.308797536917649</v>
       </c>
       <c r="Q49">
-        <v>0.32020255991575147</v>
+        <v>0.3216062366606578</v>
       </c>
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
@@ -3120,46 +3132,46 @@
         <v>18</v>
       </c>
       <c r="D50">
-        <v>68.570527268831</v>
+        <v>63.888243018283802</v>
       </c>
       <c r="E50">
-        <v>49.370779633558321</v>
+        <v>45.999534973164337</v>
       </c>
       <c r="F50">
-        <v>34.263321065689468</v>
+        <v>31.92367727137605</v>
       </c>
       <c r="G50">
-        <v>125.82115678227601</v>
+        <v>50.453771533682371</v>
       </c>
       <c r="H50">
-        <v>48.213205548500149</v>
+        <v>111.99670587608939</v>
       </c>
       <c r="I50">
         <v>10</v>
       </c>
       <c r="J50">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K50">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L50">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M50">
-        <v>0.53205676622873577</v>
+        <v>0.51347246539093006</v>
       </c>
       <c r="N50">
-        <v>2.538034477239381</v>
+        <v>2.5427288298299429</v>
       </c>
       <c r="O50">
-        <v>2.187528752869647</v>
+        <v>2.3478498220255082</v>
       </c>
       <c r="P50">
-        <v>0.30433898054297098</v>
+        <v>0.39807550198506308</v>
       </c>
       <c r="Q50">
-        <v>0.30707401556350661</v>
+        <v>0.32771464537327261</v>
       </c>
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
@@ -3173,46 +3185,46 @@
         <v>19</v>
       </c>
       <c r="D51">
-        <v>70.462746617623168</v>
+        <v>65.414191245523043</v>
       </c>
       <c r="E51">
-        <v>50.733177564688681</v>
+        <v>47.098217696776587</v>
       </c>
       <c r="F51">
-        <v>35.208825229893939</v>
+        <v>32.686163081562952</v>
       </c>
       <c r="G51">
-        <v>126.2200744429818</v>
+        <v>50.509024125002021</v>
       </c>
       <c r="H51">
-        <v>48.308399486127691</v>
+        <v>112.0781469938814</v>
       </c>
       <c r="I51">
         <v>10</v>
       </c>
       <c r="J51">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K51">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L51">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M51">
-        <v>0.53248551770066987</v>
+        <v>0.51358398306536812</v>
       </c>
       <c r="N51">
-        <v>2.4768900207114388</v>
+        <v>2.485503038761653</v>
       </c>
       <c r="O51">
-        <v>2.128784459879173</v>
+        <v>2.2930804026452898</v>
       </c>
       <c r="P51">
-        <v>0.30615512238030201</v>
+        <v>0.39861865330577551</v>
       </c>
       <c r="Q51">
-        <v>0.30689648650116802</v>
+        <v>0.32872607153999112</v>
       </c>
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
@@ -3226,46 +3238,46 @@
         <v>20</v>
       </c>
       <c r="D52">
-        <v>68.570527268831</v>
+        <v>63.888243018283802</v>
       </c>
       <c r="E52">
-        <v>49.370779633558321</v>
+        <v>45.999534973164337</v>
       </c>
       <c r="F52">
-        <v>34.263321065689468</v>
+        <v>31.92367727137605</v>
       </c>
       <c r="G52">
-        <v>125.82115678227601</v>
+        <v>50.453771533682371</v>
       </c>
       <c r="H52">
-        <v>48.213205548500149</v>
+        <v>111.99670587608939</v>
       </c>
       <c r="I52">
         <v>10</v>
       </c>
       <c r="J52">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K52">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L52">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M52">
-        <v>0.53205676622873577</v>
+        <v>0.51347246539093006</v>
       </c>
       <c r="N52">
-        <v>2.538034477239381</v>
+        <v>2.5427288298299429</v>
       </c>
       <c r="O52">
-        <v>2.187528752869647</v>
+        <v>2.3478498220255082</v>
       </c>
       <c r="P52">
-        <v>0.30433898054297098</v>
+        <v>0.39807550198506308</v>
       </c>
       <c r="Q52">
-        <v>0.30707401556350661</v>
+        <v>0.32771464537327261</v>
       </c>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
@@ -3279,46 +3291,46 @@
         <v>21</v>
       </c>
       <c r="D53">
-        <v>66.723085809212307</v>
+        <v>62.384762842299097</v>
       </c>
       <c r="E53">
-        <v>48.040621782632861</v>
+        <v>44.917029246455357</v>
       </c>
       <c r="F53">
-        <v>33.340191517147197</v>
+        <v>31.172418297040011</v>
       </c>
       <c r="G53">
-        <v>125.4348126943699</v>
+        <v>50.399914254847523</v>
       </c>
       <c r="H53">
-        <v>48.121172361128643</v>
+        <v>111.9175690269544</v>
       </c>
       <c r="I53">
         <v>10</v>
       </c>
       <c r="J53">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K53">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L53">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M53">
-        <v>0.53164060959584714</v>
+        <v>0.5133631778653317</v>
       </c>
       <c r="N53">
-        <v>2.60113846580423</v>
+        <v>2.6018770591806248</v>
       </c>
       <c r="O53">
-        <v>2.2480974640308049</v>
+        <v>2.4044332809147848</v>
       </c>
       <c r="P53">
-        <v>0.30229789983092459</v>
+        <v>0.39738812074090668</v>
       </c>
       <c r="Q53">
-        <v>0.30705671214913499</v>
+        <v>0.32653628928737721</v>
       </c>
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
@@ -3332,46 +3344,46 @@
         <v>22</v>
       </c>
       <c r="D54">
-        <v>63.154436558463011</v>
+        <v>59.442271628607038</v>
       </c>
       <c r="E54">
-        <v>45.471194322093368</v>
+        <v>42.798435572597057</v>
       </c>
       <c r="F54">
-        <v>31.55700885953279</v>
+        <v>29.702114287382361</v>
       </c>
       <c r="G54">
-        <v>124.69743125362081</v>
+        <v>50.296166526600288</v>
       </c>
       <c r="H54">
-        <v>47.945948185147991</v>
+        <v>111.7658197722923</v>
       </c>
       <c r="I54">
         <v>10</v>
       </c>
       <c r="J54">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K54">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L54">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M54">
-        <v>0.53084387124872967</v>
+        <v>0.51315100538703506</v>
       </c>
       <c r="N54">
-        <v>2.7336698551486589</v>
+        <v>2.7263760596406801</v>
       </c>
       <c r="O54">
-        <v>2.3751300490368989</v>
+        <v>2.5234567234777652</v>
       </c>
       <c r="P54">
-        <v>0.29750232122338222</v>
+        <v>0.3955555682029136</v>
       </c>
       <c r="Q54">
-        <v>0.30640925482616688</v>
+        <v>0.32364979831693519</v>
       </c>
     </row>
     <row r="55" spans="1:17" x14ac:dyDescent="0.25">
@@ -3385,46 +3397,46 @@
         <v>23</v>
       </c>
       <c r="D55">
-        <v>61.429479151733332</v>
+        <v>58.001875554335442</v>
       </c>
       <c r="E55">
-        <v>44.229224989248003</v>
+        <v>41.761350399121518</v>
       </c>
       <c r="F55">
-        <v>30.695082142538109</v>
+        <v>28.98237717699033</v>
       </c>
       <c r="G55">
-        <v>124.3452849054958</v>
+        <v>50.246174013910817</v>
       </c>
       <c r="H55">
-        <v>47.862464338082169</v>
+        <v>111.69302716806369</v>
       </c>
       <c r="I55">
         <v>10</v>
       </c>
       <c r="J55">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K55">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L55">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M55">
-        <v>0.53046226682753017</v>
+        <v>0.51304798467728085</v>
       </c>
       <c r="N55">
-        <v>2.8033405397792448</v>
+        <v>2.7919649086221678</v>
       </c>
       <c r="O55">
-        <v>2.4418243825491972</v>
+        <v>2.58612326871192</v>
       </c>
       <c r="P55">
-        <v>0.29472660246458282</v>
+        <v>0.3943965753402694</v>
       </c>
       <c r="Q55">
-        <v>0.30576337948295929</v>
+        <v>0.32192566964963731</v>
       </c>
     </row>
     <row r="56" spans="1:17" x14ac:dyDescent="0.25">
@@ -3438,46 +3450,46 @@
         <v>24</v>
       </c>
       <c r="D56">
-        <v>59.741782206948571</v>
+        <v>56.581173663985822</v>
       </c>
       <c r="E56">
-        <v>43.014083189002967</v>
+        <v>40.738445038069777</v>
       </c>
       <c r="F56">
-        <v>29.851773733168059</v>
+        <v>28.27248085642043</v>
       </c>
       <c r="G56">
-        <v>124.0034877936392</v>
+        <v>50.197372283392603</v>
       </c>
       <c r="H56">
-        <v>47.781553711995578</v>
+        <v>111.6221776587754</v>
       </c>
       <c r="I56">
         <v>10</v>
       </c>
       <c r="J56">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K56">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L56">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M56">
-        <v>0.53009120687357958</v>
+        <v>0.51294692221474292</v>
       </c>
       <c r="N56">
-        <v>2.8754589361020839</v>
+        <v>2.8599539292548628</v>
       </c>
       <c r="O56">
-        <v>2.5108055779185219</v>
+        <v>2.6510584755769342</v>
       </c>
       <c r="P56">
-        <v>0.29168335760040942</v>
+        <v>0.39306561310590821</v>
       </c>
       <c r="Q56">
-        <v>0.30489111892611392</v>
+        <v>0.3200025122659077</v>
       </c>
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
@@ -3491,46 +3503,46 @@
         <v>25</v>
       </c>
       <c r="D57">
-        <v>61.429479151733332</v>
+        <v>58.001875554335442</v>
       </c>
       <c r="E57">
-        <v>44.229224989248003</v>
+        <v>41.761350399121518</v>
       </c>
       <c r="F57">
-        <v>30.695082142538109</v>
+        <v>28.98237717699033</v>
       </c>
       <c r="G57">
-        <v>124.3452849054958</v>
+        <v>50.246174013910817</v>
       </c>
       <c r="H57">
-        <v>47.862464338082169</v>
+        <v>111.69302716806369</v>
       </c>
       <c r="I57">
         <v>10</v>
       </c>
       <c r="J57">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K57">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L57">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M57">
-        <v>0.53046226682753017</v>
+        <v>0.51304798467728085</v>
       </c>
       <c r="N57">
-        <v>2.8033405397792448</v>
+        <v>2.7919649086221678</v>
       </c>
       <c r="O57">
-        <v>2.4418243825491972</v>
+        <v>2.58612326871192</v>
       </c>
       <c r="P57">
-        <v>0.29472660246458282</v>
+        <v>0.3943965753402694</v>
       </c>
       <c r="Q57">
-        <v>0.30576337948295929</v>
+        <v>0.32192566964963731</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
@@ -3544,46 +3556,46 @@
         <v>26</v>
       </c>
       <c r="D58">
-        <v>61.429479151733332</v>
+        <v>58.001875554335442</v>
       </c>
       <c r="E58">
-        <v>44.229224989248003</v>
+        <v>41.761350399121518</v>
       </c>
       <c r="F58">
-        <v>30.695082142538109</v>
+        <v>28.98237717699033</v>
       </c>
       <c r="G58">
-        <v>124.3452849054958</v>
+        <v>50.246174013910817</v>
       </c>
       <c r="H58">
-        <v>47.862464338082169</v>
+        <v>111.69302716806369</v>
       </c>
       <c r="I58">
         <v>10</v>
       </c>
       <c r="J58">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K58">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L58">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M58">
-        <v>0.53046226682753017</v>
+        <v>0.51304798467728085</v>
       </c>
       <c r="N58">
-        <v>2.8033405397792448</v>
+        <v>2.7919649086221678</v>
       </c>
       <c r="O58">
-        <v>2.4418243825491972</v>
+        <v>2.58612326871192</v>
       </c>
       <c r="P58">
-        <v>0.29472660246458282</v>
+        <v>0.3943965753402694</v>
       </c>
       <c r="Q58">
-        <v>0.30576337948295929</v>
+        <v>0.32192566964963731</v>
       </c>
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
@@ -3597,46 +3609,46 @@
         <v>27</v>
       </c>
       <c r="D59">
-        <v>63.154436558463011</v>
+        <v>59.442271628607038</v>
       </c>
       <c r="E59">
-        <v>45.471194322093368</v>
+        <v>42.798435572597057</v>
       </c>
       <c r="F59">
-        <v>31.55700885953279</v>
+        <v>29.702114287382361</v>
       </c>
       <c r="G59">
-        <v>124.69743125362081</v>
+        <v>50.296166526600288</v>
       </c>
       <c r="H59">
-        <v>47.945948185147991</v>
+        <v>111.7658197722923</v>
       </c>
       <c r="I59">
         <v>10</v>
       </c>
       <c r="J59">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K59">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L59">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M59">
-        <v>0.53084387124872967</v>
+        <v>0.51315100538703506</v>
       </c>
       <c r="N59">
-        <v>2.7336698551486589</v>
+        <v>2.7263760596406801</v>
       </c>
       <c r="O59">
-        <v>2.3751300490368989</v>
+        <v>2.5234567234777652</v>
       </c>
       <c r="P59">
-        <v>0.29750232122338222</v>
+        <v>0.3955555682029136</v>
       </c>
       <c r="Q59">
-        <v>0.30640925482616688</v>
+        <v>0.32364979831693519</v>
       </c>
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
@@ -3650,46 +3662,46 @@
         <v>28</v>
       </c>
       <c r="D60">
-        <v>64.918366246852145</v>
+        <v>60.903008519827928</v>
       </c>
       <c r="E60">
-        <v>46.741223697733538</v>
+        <v>43.850166134276108</v>
       </c>
       <c r="F60">
-        <v>32.438409246227067</v>
+        <v>30.432015297187611</v>
       </c>
       <c r="G60">
-        <v>125.0604285515934</v>
+        <v>50.347396741392451</v>
       </c>
       <c r="H60">
-        <v>48.032137099440767</v>
+        <v>111.84063791718761</v>
       </c>
       <c r="I60">
         <v>10</v>
       </c>
       <c r="J60">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K60">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L60">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M60">
-        <v>0.53123648693348835</v>
+        <v>0.51325604768208211</v>
       </c>
       <c r="N60">
-        <v>2.6663111790714131</v>
+        <v>2.6630545616769861</v>
       </c>
       <c r="O60">
-        <v>2.3105941919367599</v>
+        <v>2.4629325159062572</v>
       </c>
       <c r="P60">
-        <v>0.30002241528958712</v>
+        <v>0.39655035709514957</v>
       </c>
       <c r="Q60">
-        <v>0.30683763730518587</v>
+        <v>0.32518390069663528</v>
       </c>
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
@@ -3703,46 +3715,46 @@
         <v>29</v>
       </c>
       <c r="D61">
-        <v>66.723085809212307</v>
+        <v>62.384762842299097</v>
       </c>
       <c r="E61">
-        <v>48.040621782632861</v>
+        <v>44.917029246455357</v>
       </c>
       <c r="F61">
-        <v>33.340191517147197</v>
+        <v>31.172418297040011</v>
       </c>
       <c r="G61">
-        <v>125.4348126943699</v>
+        <v>50.399914254847523</v>
       </c>
       <c r="H61">
-        <v>48.121172361128643</v>
+        <v>111.9175690269544</v>
       </c>
       <c r="I61">
         <v>10</v>
       </c>
       <c r="J61">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="K61">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L61">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="M61">
-        <v>0.53164060959584714</v>
+        <v>0.5133631778653317</v>
       </c>
       <c r="N61">
-        <v>2.60113846580423</v>
+        <v>2.6018770591806248</v>
       </c>
       <c r="O61">
-        <v>2.2480974640308049</v>
+        <v>2.4044332809147848</v>
       </c>
       <c r="P61">
-        <v>0.30229789983092459</v>
+        <v>0.39738812074090668</v>
       </c>
       <c r="Q61">
-        <v>0.30705671214913499</v>
+        <v>0.32653628928737721</v>
       </c>
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
@@ -3756,46 +3768,46 @@
         <v>18</v>
       </c>
       <c r="D62">
-        <v>62.795303826198541</v>
+        <v>65.417649009978234</v>
       </c>
       <c r="E62">
-        <v>45.212618754862952</v>
+        <v>47.100707287184328</v>
       </c>
       <c r="F62">
-        <v>31.37755741587489</v>
+        <v>32.687890857305931</v>
       </c>
       <c r="G62">
-        <v>48.010533733957637</v>
+        <v>119.4188407022428</v>
       </c>
       <c r="H62">
-        <v>109.45643709907981</v>
+        <v>47.181613456933277</v>
       </c>
       <c r="I62">
         <v>10</v>
       </c>
       <c r="J62">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K62">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L62">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M62">
-        <v>0.50605481461525192</v>
+        <v>0.52219352782079764</v>
       </c>
       <c r="N62">
-        <v>2.5076233609581058</v>
+        <v>2.546720291549522</v>
       </c>
       <c r="O62">
-        <v>2.388713659466668</v>
+        <v>2.2929591978629551</v>
       </c>
       <c r="P62">
-        <v>0.39338422835282361</v>
+        <v>0.3061446329919425</v>
       </c>
       <c r="Q62">
-        <v>0.33283078183203041</v>
+        <v>0.32089401057272721</v>
       </c>
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
@@ -3809,46 +3821,46 @@
         <v>19</v>
       </c>
       <c r="D63">
-        <v>64.17495964201855</v>
+        <v>67.078556952777859</v>
       </c>
       <c r="E63">
-        <v>46.205970942253352</v>
+        <v>48.296561006000061</v>
       </c>
       <c r="F63">
-        <v>32.066943833923823</v>
+        <v>33.517813338164054</v>
       </c>
       <c r="G63">
-        <v>48.025838474226212</v>
+        <v>119.67472060686011</v>
       </c>
       <c r="H63">
-        <v>109.4805602195615</v>
+        <v>47.249326341937604</v>
       </c>
       <c r="I63">
         <v>10</v>
       </c>
       <c r="J63">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K63">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L63">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M63">
-        <v>0.50608216700222231</v>
+        <v>0.52242760720006809</v>
       </c>
       <c r="N63">
-        <v>2.4543279742190971</v>
+        <v>2.4884859563438329</v>
       </c>
       <c r="O63">
-        <v>2.3373602544782521</v>
+        <v>2.236184062599877</v>
       </c>
       <c r="P63">
-        <v>0.39441736192231369</v>
+        <v>0.30834980686732699</v>
       </c>
       <c r="Q63">
-        <v>0.3344907450608553</v>
+        <v>0.32140333230003237</v>
       </c>
     </row>
     <row r="64" spans="1:17" x14ac:dyDescent="0.25">
@@ -3862,46 +3874,46 @@
         <v>20</v>
       </c>
       <c r="D64">
-        <v>62.795303826198541</v>
+        <v>65.417649009978234</v>
       </c>
       <c r="E64">
-        <v>45.212618754862952</v>
+        <v>47.100707287184328</v>
       </c>
       <c r="F64">
-        <v>31.37755741587489</v>
+        <v>32.687890857305931</v>
       </c>
       <c r="G64">
-        <v>48.010533733957637</v>
+        <v>119.4188407022428</v>
       </c>
       <c r="H64">
-        <v>109.45643709907981</v>
+        <v>47.181613456933277</v>
       </c>
       <c r="I64">
         <v>10</v>
       </c>
       <c r="J64">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K64">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L64">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M64">
-        <v>0.50605481461525192</v>
+        <v>0.52219352782079764</v>
       </c>
       <c r="N64">
-        <v>2.5076233609581058</v>
+        <v>2.546720291549522</v>
       </c>
       <c r="O64">
-        <v>2.388713659466668</v>
+        <v>2.2929591978629551</v>
       </c>
       <c r="P64">
-        <v>0.39338422835282361</v>
+        <v>0.3061446329919425</v>
       </c>
       <c r="Q64">
-        <v>0.33283078183203041</v>
+        <v>0.32089401057272721</v>
       </c>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
@@ -3915,46 +3927,46 @@
         <v>21</v>
       </c>
       <c r="D65">
-        <v>61.427572295570783</v>
+        <v>63.787840732247993</v>
       </c>
       <c r="E65">
-        <v>44.227852052810967</v>
+        <v>45.92724532721855</v>
       </c>
       <c r="F65">
-        <v>30.69412932465081</v>
+        <v>31.873508257089679</v>
       </c>
       <c r="G65">
-        <v>47.99547335066908</v>
+        <v>119.16996704243761</v>
       </c>
       <c r="H65">
-        <v>109.4327566661816</v>
+        <v>47.115867699615677</v>
       </c>
       <c r="I65">
         <v>10</v>
       </c>
       <c r="J65">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K65">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L65">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M65">
-        <v>0.50602776313011433</v>
+        <v>0.52196523933676098</v>
       </c>
       <c r="N65">
-        <v>2.5628268240742762</v>
+        <v>2.6068578718637729</v>
       </c>
       <c r="O65">
-        <v>2.4419001825148761</v>
+        <v>2.351545345916803</v>
       </c>
       <c r="P65">
-        <v>0.39223509156839692</v>
+        <v>0.30372978986510951</v>
       </c>
       <c r="Q65">
-        <v>0.33103199706833281</v>
+        <v>0.32020255991575147</v>
       </c>
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
@@ -3968,46 +3980,46 @@
         <v>22</v>
       </c>
       <c r="D66">
-        <v>58.72714627397594</v>
+        <v>60.616656149042228</v>
       </c>
       <c r="E66">
-        <v>42.283545317262679</v>
+        <v>43.643992427310401</v>
       </c>
       <c r="F66">
-        <v>29.344780450180291</v>
+        <v>30.288930744553419</v>
       </c>
       <c r="G66">
-        <v>47.966060543759433</v>
+        <v>118.69205806099301</v>
       </c>
       <c r="H66">
-        <v>109.38667506904341</v>
+        <v>46.9899295195438</v>
       </c>
       <c r="I66">
         <v>10</v>
       </c>
       <c r="J66">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K66">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L66">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M66">
-        <v>0.50597453978812246</v>
+        <v>0.52152515692786794</v>
       </c>
       <c r="N66">
-        <v>2.6793867163017819</v>
+        <v>2.7332749462979842</v>
       </c>
       <c r="O66">
-        <v>2.5541850663101311</v>
+        <v>2.474567380146885</v>
       </c>
       <c r="P66">
-        <v>0.38956349472274682</v>
+        <v>0.29823367213557822</v>
       </c>
       <c r="Q66">
-        <v>0.32698781275712452</v>
+        <v>0.31824478662720979</v>
       </c>
     </row>
     <row r="67" spans="1:17" x14ac:dyDescent="0.25">
@@ -4021,46 +4033,46 @@
         <v>23</v>
       </c>
       <c r="D67">
-        <v>57.394098326113337</v>
+        <v>59.073001990560023</v>
       </c>
       <c r="E67">
-        <v>41.323750794801597</v>
+        <v>42.532561433203213</v>
       </c>
       <c r="F67">
-        <v>28.678683051592309</v>
+        <v>29.517597634643032</v>
       </c>
       <c r="G67">
-        <v>47.951696072412403</v>
+        <v>118.4624734194721</v>
       </c>
       <c r="H67">
-        <v>109.3642505253079</v>
+        <v>46.929575505113263</v>
       </c>
       <c r="I67">
         <v>10</v>
       </c>
       <c r="J67">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K67">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L67">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M67">
-        <v>0.5059483567878873</v>
+        <v>0.52131295209185735</v>
       </c>
       <c r="N67">
-        <v>2.7409777518212919</v>
+        <v>2.7997908240894098</v>
       </c>
       <c r="O67">
-        <v>2.6135091302889681</v>
+        <v>2.539231035253132</v>
       </c>
       <c r="P67">
-        <v>0.38802713982643561</v>
+        <v>0.2951318234086634</v>
       </c>
       <c r="Q67">
-        <v>0.32472586731708869</v>
+        <v>0.31696271150964378</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
@@ -4074,46 +4086,46 @@
         <v>24</v>
       </c>
       <c r="D68">
-        <v>56.072267379004629</v>
+        <v>57.555883754216318</v>
       </c>
       <c r="E68">
-        <v>40.37203251288333</v>
+        <v>41.440236303035753</v>
       </c>
       <c r="F68">
-        <v>28.01819056394103</v>
+        <v>28.759523994306811</v>
       </c>
       <c r="G68">
-        <v>47.937551845002439</v>
+        <v>118.238794121193</v>
       </c>
       <c r="H68">
-        <v>109.3422218737924</v>
+        <v>46.870864730574567</v>
       </c>
       <c r="I68">
         <v>10</v>
       </c>
       <c r="J68">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K68">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L68">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M68">
-        <v>0.50592245239155786</v>
+        <v>0.52110571487161983</v>
       </c>
       <c r="N68">
-        <v>2.8049476340185548</v>
+        <v>2.8686842783414348</v>
       </c>
       <c r="O68">
-        <v>2.675119216886976</v>
+        <v>2.6061627450731581</v>
       </c>
       <c r="P68">
-        <v>0.38634689668466637</v>
+        <v>0.29177901560962272</v>
       </c>
       <c r="Q68">
-        <v>0.32229189547365128</v>
+        <v>0.31546689122119281</v>
       </c>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
@@ -4127,46 +4139,46 @@
         <v>25</v>
       </c>
       <c r="D69">
-        <v>57.394098326113337</v>
+        <v>59.073001990560023</v>
       </c>
       <c r="E69">
-        <v>41.323750794801597</v>
+        <v>42.532561433203213</v>
       </c>
       <c r="F69">
-        <v>28.678683051592309</v>
+        <v>29.517597634643032</v>
       </c>
       <c r="G69">
-        <v>47.951696072412403</v>
+        <v>118.4624734194721</v>
       </c>
       <c r="H69">
-        <v>109.3642505253079</v>
+        <v>46.929575505113263</v>
       </c>
       <c r="I69">
         <v>10</v>
       </c>
       <c r="J69">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K69">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L69">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M69">
-        <v>0.5059483567878873</v>
+        <v>0.52131295209185735</v>
       </c>
       <c r="N69">
-        <v>2.7409777518212919</v>
+        <v>2.7997908240894098</v>
       </c>
       <c r="O69">
-        <v>2.6135091302889681</v>
+        <v>2.539231035253132</v>
       </c>
       <c r="P69">
-        <v>0.38802713982643561</v>
+        <v>0.2951318234086634</v>
       </c>
       <c r="Q69">
-        <v>0.32472586731708869</v>
+        <v>0.31696271150964378</v>
       </c>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
@@ -4180,46 +4192,46 @@
         <v>26</v>
       </c>
       <c r="D70">
-        <v>57.394098326113337</v>
+        <v>59.073001990560023</v>
       </c>
       <c r="E70">
-        <v>41.323750794801597</v>
+        <v>42.532561433203213</v>
       </c>
       <c r="F70">
-        <v>28.678683051592309</v>
+        <v>29.517597634643032</v>
       </c>
       <c r="G70">
-        <v>47.951696072412403</v>
+        <v>118.4624734194721</v>
       </c>
       <c r="H70">
-        <v>109.3642505253079</v>
+        <v>46.929575505113263</v>
       </c>
       <c r="I70">
         <v>10</v>
       </c>
       <c r="J70">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K70">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L70">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M70">
-        <v>0.5059483567878873</v>
+        <v>0.52131295209185735</v>
       </c>
       <c r="N70">
-        <v>2.7409777518212919</v>
+        <v>2.7997908240894098</v>
       </c>
       <c r="O70">
-        <v>2.6135091302889681</v>
+        <v>2.539231035253132</v>
       </c>
       <c r="P70">
-        <v>0.38802713982643561</v>
+        <v>0.2951318234086634</v>
       </c>
       <c r="Q70">
-        <v>0.32472586731708869</v>
+        <v>0.31696271150964378</v>
       </c>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
@@ -4233,46 +4245,46 @@
         <v>27</v>
       </c>
       <c r="D71">
-        <v>58.72714627397594</v>
+        <v>60.616656149042228</v>
       </c>
       <c r="E71">
-        <v>42.283545317262679</v>
+        <v>43.643992427310401</v>
       </c>
       <c r="F71">
-        <v>29.344780450180291</v>
+        <v>30.288930744553419</v>
       </c>
       <c r="G71">
-        <v>47.966060543759433</v>
+        <v>118.69205806099301</v>
       </c>
       <c r="H71">
-        <v>109.38667506904341</v>
+        <v>46.9899295195438</v>
       </c>
       <c r="I71">
         <v>10</v>
       </c>
       <c r="J71">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K71">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L71">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M71">
-        <v>0.50597453978812246</v>
+        <v>0.52152515692786794</v>
       </c>
       <c r="N71">
-        <v>2.6793867163017819</v>
+        <v>2.7332749462979842</v>
       </c>
       <c r="O71">
-        <v>2.5541850663101311</v>
+        <v>2.474567380146885</v>
       </c>
       <c r="P71">
-        <v>0.38956349472274682</v>
+        <v>0.29823367213557822</v>
       </c>
       <c r="Q71">
-        <v>0.32698781275712452</v>
+        <v>0.31824478662720979</v>
       </c>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
@@ -4286,46 +4298,46 @@
         <v>28</v>
       </c>
       <c r="D72">
-        <v>60.071579632223923</v>
+        <v>62.187899379591968</v>
       </c>
       <c r="E72">
-        <v>43.25153733520122</v>
+        <v>44.775287553306221</v>
       </c>
       <c r="F72">
-        <v>30.016566910629649</v>
+        <v>31.07404956199451</v>
       </c>
       <c r="G72">
-        <v>47.980650994985048</v>
+        <v>118.92780032253449</v>
       </c>
       <c r="H72">
-        <v>109.4095066190325</v>
+        <v>47.052000777818073</v>
       </c>
       <c r="I72">
         <v>10</v>
       </c>
       <c r="J72">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K72">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L72">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M72">
-        <v>0.50600100673741177</v>
+        <v>0.52174251932526505</v>
       </c>
       <c r="N72">
-        <v>2.6200435976148282</v>
+        <v>2.6690047864009649</v>
       </c>
       <c r="O72">
-        <v>2.4970210691702239</v>
+        <v>2.4120448109109969</v>
       </c>
       <c r="P72">
-        <v>0.39096374245575077</v>
+        <v>0.30109610109210211</v>
       </c>
       <c r="Q72">
-        <v>0.32908699495948213</v>
+        <v>0.31932200476969269</v>
       </c>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
@@ -4339,49 +4351,1958 @@
         <v>29</v>
       </c>
       <c r="D73">
+        <v>63.787840732247993</v>
+      </c>
+      <c r="E73">
+        <v>45.92724532721855</v>
+      </c>
+      <c r="F73">
+        <v>31.873508257089679</v>
+      </c>
+      <c r="G73">
+        <v>119.16996704243761</v>
+      </c>
+      <c r="H73">
+        <v>47.115867699615677</v>
+      </c>
+      <c r="I73">
+        <v>10</v>
+      </c>
+      <c r="J73">
+        <v>10</v>
+      </c>
+      <c r="K73">
+        <v>10</v>
+      </c>
+      <c r="L73">
+        <v>0.3</v>
+      </c>
+      <c r="M73">
+        <v>0.52196523933676098</v>
+      </c>
+      <c r="N73">
+        <v>2.6068578718637729</v>
+      </c>
+      <c r="O73">
+        <v>2.351545345916803</v>
+      </c>
+      <c r="P73">
+        <v>0.30372978986510951</v>
+      </c>
+      <c r="Q73">
+        <v>0.32020255991575147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>35</v>
+      </c>
+      <c r="B74">
+        <v>29</v>
+      </c>
+      <c r="C74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74">
+        <v>62.795303826198541</v>
+      </c>
+      <c r="E74">
+        <v>45.212618754862952</v>
+      </c>
+      <c r="F74">
+        <v>31.37755741587489</v>
+      </c>
+      <c r="G74">
+        <v>48.010533733957637</v>
+      </c>
+      <c r="H74">
+        <v>109.45643709907981</v>
+      </c>
+      <c r="I74">
+        <v>10</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0.7</v>
+      </c>
+      <c r="M74">
+        <v>0.50605481461525192</v>
+      </c>
+      <c r="N74">
+        <v>2.5076233609581058</v>
+      </c>
+      <c r="O74">
+        <v>2.388713659466668</v>
+      </c>
+      <c r="P74">
+        <v>0.39338422835282361</v>
+      </c>
+      <c r="Q74">
+        <v>0.33283078183203041</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>35</v>
+      </c>
+      <c r="B75">
+        <v>30</v>
+      </c>
+      <c r="C75" t="s">
+        <v>19</v>
+      </c>
+      <c r="D75">
+        <v>64.17495964201855</v>
+      </c>
+      <c r="E75">
+        <v>46.205970942253352</v>
+      </c>
+      <c r="F75">
+        <v>32.066943833923823</v>
+      </c>
+      <c r="G75">
+        <v>48.025838474226212</v>
+      </c>
+      <c r="H75">
+        <v>109.4805602195615</v>
+      </c>
+      <c r="I75">
+        <v>10</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0.7</v>
+      </c>
+      <c r="M75">
+        <v>0.50608216700222231</v>
+      </c>
+      <c r="N75">
+        <v>2.4543279742190971</v>
+      </c>
+      <c r="O75">
+        <v>2.3373602544782521</v>
+      </c>
+      <c r="P75">
+        <v>0.39441736192231369</v>
+      </c>
+      <c r="Q75">
+        <v>0.3344907450608553</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76">
+        <v>29</v>
+      </c>
+      <c r="C76" t="s">
+        <v>20</v>
+      </c>
+      <c r="D76">
+        <v>62.795303826198541</v>
+      </c>
+      <c r="E76">
+        <v>45.212618754862952</v>
+      </c>
+      <c r="F76">
+        <v>31.37755741587489</v>
+      </c>
+      <c r="G76">
+        <v>48.010533733957637</v>
+      </c>
+      <c r="H76">
+        <v>109.45643709907981</v>
+      </c>
+      <c r="I76">
+        <v>10</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+      <c r="K76">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0.7</v>
+      </c>
+      <c r="M76">
+        <v>0.50605481461525192</v>
+      </c>
+      <c r="N76">
+        <v>2.5076233609581058</v>
+      </c>
+      <c r="O76">
+        <v>2.388713659466668</v>
+      </c>
+      <c r="P76">
+        <v>0.39338422835282361</v>
+      </c>
+      <c r="Q76">
+        <v>0.33283078183203041</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>35</v>
+      </c>
+      <c r="B77">
+        <v>28</v>
+      </c>
+      <c r="C77" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77">
         <v>61.427572295570783</v>
       </c>
-      <c r="E73">
+      <c r="E77">
         <v>44.227852052810967</v>
       </c>
-      <c r="F73">
+      <c r="F77">
         <v>30.69412932465081</v>
       </c>
-      <c r="G73">
+      <c r="G77">
         <v>47.99547335066908</v>
       </c>
-      <c r="H73">
+      <c r="H77">
         <v>109.4327566661816</v>
       </c>
-      <c r="I73">
-        <v>10</v>
-      </c>
-      <c r="J73">
-        <v>0</v>
-      </c>
-      <c r="K73">
-        <v>0</v>
-      </c>
-      <c r="L73">
+      <c r="I77">
+        <v>10</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+      <c r="K77">
+        <v>0</v>
+      </c>
+      <c r="L77">
         <v>0.7</v>
       </c>
-      <c r="M73">
+      <c r="M77">
         <v>0.50602776313011433</v>
       </c>
-      <c r="N73">
+      <c r="N77">
         <v>2.5628268240742762</v>
       </c>
-      <c r="O73">
+      <c r="O77">
         <v>2.4419001825148761</v>
       </c>
-      <c r="P73">
+      <c r="P77">
         <v>0.39223509156839692</v>
       </c>
-      <c r="Q73">
+      <c r="Q77">
         <v>0.33103199706833281</v>
       </c>
     </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78">
+        <v>26</v>
+      </c>
+      <c r="C78" t="s">
+        <v>22</v>
+      </c>
+      <c r="D78">
+        <v>58.72714627397594</v>
+      </c>
+      <c r="E78">
+        <v>42.283545317262679</v>
+      </c>
+      <c r="F78">
+        <v>29.344780450180291</v>
+      </c>
+      <c r="G78">
+        <v>47.966060543759433</v>
+      </c>
+      <c r="H78">
+        <v>109.38667506904341</v>
+      </c>
+      <c r="I78">
+        <v>10</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0.7</v>
+      </c>
+      <c r="M78">
+        <v>0.50597453978812246</v>
+      </c>
+      <c r="N78">
+        <v>2.6793867163017819</v>
+      </c>
+      <c r="O78">
+        <v>2.5541850663101311</v>
+      </c>
+      <c r="P78">
+        <v>0.38956349472274682</v>
+      </c>
+      <c r="Q78">
+        <v>0.32698781275712452</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>35</v>
+      </c>
+      <c r="B79">
+        <v>25</v>
+      </c>
+      <c r="C79" t="s">
+        <v>23</v>
+      </c>
+      <c r="D79">
+        <v>57.394098326113337</v>
+      </c>
+      <c r="E79">
+        <v>41.323750794801597</v>
+      </c>
+      <c r="F79">
+        <v>28.678683051592309</v>
+      </c>
+      <c r="G79">
+        <v>47.951696072412403</v>
+      </c>
+      <c r="H79">
+        <v>109.3642505253079</v>
+      </c>
+      <c r="I79">
+        <v>10</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+      <c r="K79">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>0.7</v>
+      </c>
+      <c r="M79">
+        <v>0.5059483567878873</v>
+      </c>
+      <c r="N79">
+        <v>2.7409777518212919</v>
+      </c>
+      <c r="O79">
+        <v>2.6135091302889681</v>
+      </c>
+      <c r="P79">
+        <v>0.38802713982643561</v>
+      </c>
+      <c r="Q79">
+        <v>0.32472586731708869</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80">
+        <v>24</v>
+      </c>
+      <c r="C80" t="s">
+        <v>24</v>
+      </c>
+      <c r="D80">
+        <v>56.072267379004629</v>
+      </c>
+      <c r="E80">
+        <v>40.37203251288333</v>
+      </c>
+      <c r="F80">
+        <v>28.01819056394103</v>
+      </c>
+      <c r="G80">
+        <v>47.937551845002439</v>
+      </c>
+      <c r="H80">
+        <v>109.3422218737924</v>
+      </c>
+      <c r="I80">
+        <v>10</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>0.7</v>
+      </c>
+      <c r="M80">
+        <v>0.50592245239155786</v>
+      </c>
+      <c r="N80">
+        <v>2.8049476340185548</v>
+      </c>
+      <c r="O80">
+        <v>2.675119216886976</v>
+      </c>
+      <c r="P80">
+        <v>0.38634689668466637</v>
+      </c>
+      <c r="Q80">
+        <v>0.32229189547365128</v>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81">
+        <v>25</v>
+      </c>
+      <c r="C81" t="s">
+        <v>25</v>
+      </c>
+      <c r="D81">
+        <v>57.394098326113337</v>
+      </c>
+      <c r="E81">
+        <v>41.323750794801597</v>
+      </c>
+      <c r="F81">
+        <v>28.678683051592309</v>
+      </c>
+      <c r="G81">
+        <v>47.951696072412403</v>
+      </c>
+      <c r="H81">
+        <v>109.3642505253079</v>
+      </c>
+      <c r="I81">
+        <v>10</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+      <c r="K81">
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <v>0.7</v>
+      </c>
+      <c r="M81">
+        <v>0.5059483567878873</v>
+      </c>
+      <c r="N81">
+        <v>2.7409777518212919</v>
+      </c>
+      <c r="O81">
+        <v>2.6135091302889681</v>
+      </c>
+      <c r="P81">
+        <v>0.38802713982643561</v>
+      </c>
+      <c r="Q81">
+        <v>0.32472586731708869</v>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82">
+        <v>25</v>
+      </c>
+      <c r="C82" t="s">
+        <v>26</v>
+      </c>
+      <c r="D82">
+        <v>57.394098326113337</v>
+      </c>
+      <c r="E82">
+        <v>41.323750794801597</v>
+      </c>
+      <c r="F82">
+        <v>28.678683051592309</v>
+      </c>
+      <c r="G82">
+        <v>47.951696072412403</v>
+      </c>
+      <c r="H82">
+        <v>109.3642505253079</v>
+      </c>
+      <c r="I82">
+        <v>10</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+      <c r="K82">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0.7</v>
+      </c>
+      <c r="M82">
+        <v>0.5059483567878873</v>
+      </c>
+      <c r="N82">
+        <v>2.7409777518212919</v>
+      </c>
+      <c r="O82">
+        <v>2.6135091302889681</v>
+      </c>
+      <c r="P82">
+        <v>0.38802713982643561</v>
+      </c>
+      <c r="Q82">
+        <v>0.32472586731708869</v>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>35</v>
+      </c>
+      <c r="B83">
+        <v>26</v>
+      </c>
+      <c r="C83" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83">
+        <v>58.72714627397594</v>
+      </c>
+      <c r="E83">
+        <v>42.283545317262679</v>
+      </c>
+      <c r="F83">
+        <v>29.344780450180291</v>
+      </c>
+      <c r="G83">
+        <v>47.966060543759433</v>
+      </c>
+      <c r="H83">
+        <v>109.38667506904341</v>
+      </c>
+      <c r="I83">
+        <v>10</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>0.7</v>
+      </c>
+      <c r="M83">
+        <v>0.50597453978812246</v>
+      </c>
+      <c r="N83">
+        <v>2.6793867163017819</v>
+      </c>
+      <c r="O83">
+        <v>2.5541850663101311</v>
+      </c>
+      <c r="P83">
+        <v>0.38956349472274682</v>
+      </c>
+      <c r="Q83">
+        <v>0.32698781275712452</v>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>35</v>
+      </c>
+      <c r="B84">
+        <v>27</v>
+      </c>
+      <c r="C84" t="s">
+        <v>28</v>
+      </c>
+      <c r="D84">
+        <v>60.071579632223923</v>
+      </c>
+      <c r="E84">
+        <v>43.25153733520122</v>
+      </c>
+      <c r="F84">
+        <v>30.016566910629649</v>
+      </c>
+      <c r="G84">
+        <v>47.980650994985048</v>
+      </c>
+      <c r="H84">
+        <v>109.4095066190325</v>
+      </c>
+      <c r="I84">
+        <v>10</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0.7</v>
+      </c>
+      <c r="M84">
+        <v>0.50600100673741177</v>
+      </c>
+      <c r="N84">
+        <v>2.6200435976148282</v>
+      </c>
+      <c r="O84">
+        <v>2.4970210691702239</v>
+      </c>
+      <c r="P84">
+        <v>0.39096374245575077</v>
+      </c>
+      <c r="Q84">
+        <v>0.32908699495948213</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>35</v>
+      </c>
+      <c r="B85">
+        <v>28</v>
+      </c>
+      <c r="C85" t="s">
+        <v>29</v>
+      </c>
+      <c r="D85">
+        <v>61.427572295570783</v>
+      </c>
+      <c r="E85">
+        <v>44.227852052810967</v>
+      </c>
+      <c r="F85">
+        <v>30.69412932465081</v>
+      </c>
+      <c r="G85">
+        <v>47.99547335066908</v>
+      </c>
+      <c r="H85">
+        <v>109.4327566661816</v>
+      </c>
+      <c r="I85">
+        <v>10</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0.7</v>
+      </c>
+      <c r="M85">
+        <v>0.50602776313011433</v>
+      </c>
+      <c r="N85">
+        <v>2.5628268240742762</v>
+      </c>
+      <c r="O85">
+        <v>2.4419001825148761</v>
+      </c>
+      <c r="P85">
+        <v>0.39223509156839692</v>
+      </c>
+      <c r="Q85">
+        <v>0.33103199706833281</v>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>36</v>
+      </c>
+      <c r="B86">
+        <v>29</v>
+      </c>
+      <c r="C86" t="s">
+        <v>18</v>
+      </c>
+      <c r="D86">
+        <v>72.887479502117856</v>
+      </c>
+      <c r="E86">
+        <v>52.478985241524853</v>
+      </c>
+      <c r="F86">
+        <v>36.420415757618251</v>
+      </c>
+      <c r="G86">
+        <v>125.57643465146499</v>
+      </c>
+      <c r="H86">
+        <v>49.056787716366919</v>
+      </c>
+      <c r="I86">
+        <v>10</v>
+      </c>
+      <c r="J86">
+        <v>10</v>
+      </c>
+      <c r="K86">
+        <v>10</v>
+      </c>
+      <c r="L86">
+        <v>0.3</v>
+      </c>
+      <c r="M86">
+        <v>0.52613343101696786</v>
+      </c>
+      <c r="N86">
+        <v>2.395928951868306</v>
+      </c>
+      <c r="O86">
+        <v>2.057966622314626</v>
+      </c>
+      <c r="P86">
+        <v>0.28754775836832791</v>
+      </c>
+      <c r="Q86">
+        <v>0.28803111012923149</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87">
+        <v>30</v>
+      </c>
+      <c r="C87" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87">
+        <v>75.015432206699501</v>
+      </c>
+      <c r="E87">
+        <v>54.011111188823641</v>
+      </c>
+      <c r="F87">
+        <v>37.483711165043609</v>
+      </c>
+      <c r="G87">
+        <v>126.06683870648909</v>
+      </c>
+      <c r="H87">
+        <v>49.196270035514523</v>
+      </c>
+      <c r="I87">
+        <v>10</v>
+      </c>
+      <c r="J87">
+        <v>10</v>
+      </c>
+      <c r="K87">
+        <v>10</v>
+      </c>
+      <c r="L87">
+        <v>0.3</v>
+      </c>
+      <c r="M87">
+        <v>0.52652536269263095</v>
+      </c>
+      <c r="N87">
+        <v>2.3363607138739</v>
+      </c>
+      <c r="O87">
+        <v>1.9995885591472169</v>
+      </c>
+      <c r="P87">
+        <v>0.28902887425931401</v>
+      </c>
+      <c r="Q87">
+        <v>0.28742817341611321</v>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>36</v>
+      </c>
+      <c r="B88">
+        <v>29</v>
+      </c>
+      <c r="C88" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88">
+        <v>72.887479502117856</v>
+      </c>
+      <c r="E88">
+        <v>52.478985241524853</v>
+      </c>
+      <c r="F88">
+        <v>36.420415757618251</v>
+      </c>
+      <c r="G88">
+        <v>125.57643465146499</v>
+      </c>
+      <c r="H88">
+        <v>49.056787716366919</v>
+      </c>
+      <c r="I88">
+        <v>10</v>
+      </c>
+      <c r="J88">
+        <v>10</v>
+      </c>
+      <c r="K88">
+        <v>10</v>
+      </c>
+      <c r="L88">
+        <v>0.3</v>
+      </c>
+      <c r="M88">
+        <v>0.52613343101696786</v>
+      </c>
+      <c r="N88">
+        <v>2.395928951868306</v>
+      </c>
+      <c r="O88">
+        <v>2.057966622314626</v>
+      </c>
+      <c r="P88">
+        <v>0.28754775836832791</v>
+      </c>
+      <c r="Q88">
+        <v>0.28803111012923149</v>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>36</v>
+      </c>
+      <c r="B89">
+        <v>28</v>
+      </c>
+      <c r="C89" t="s">
+        <v>21</v>
+      </c>
+      <c r="D89">
+        <v>70.820362129811755</v>
+      </c>
+      <c r="E89">
+        <v>50.990660733464459</v>
+      </c>
+      <c r="F89">
+        <v>35.387518549024328</v>
+      </c>
+      <c r="G89">
+        <v>125.10629968854499</v>
+      </c>
+      <c r="H89">
+        <v>48.923519696935983</v>
+      </c>
+      <c r="I89">
+        <v>10</v>
+      </c>
+      <c r="J89">
+        <v>10</v>
+      </c>
+      <c r="K89">
+        <v>10</v>
+      </c>
+      <c r="L89">
+        <v>0.3</v>
+      </c>
+      <c r="M89">
+        <v>0.5257551807881673</v>
+      </c>
+      <c r="N89">
+        <v>2.457341563242633</v>
+      </c>
+      <c r="O89">
+        <v>2.118034919463617</v>
+      </c>
+      <c r="P89">
+        <v>0.2858400807349698</v>
+      </c>
+      <c r="Q89">
+        <v>0.28842336896168908</v>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>36</v>
+      </c>
+      <c r="B90">
+        <v>26</v>
+      </c>
+      <c r="C90" t="s">
+        <v>22</v>
+      </c>
+      <c r="D90">
+        <v>66.85524692559936</v>
+      </c>
+      <c r="E90">
+        <v>48.135777786431532</v>
+      </c>
+      <c r="F90">
+        <v>33.406229783783488</v>
+      </c>
+      <c r="G90">
+        <v>124.2218269962178</v>
+      </c>
+      <c r="H90">
+        <v>48.674021953782614</v>
+      </c>
+      <c r="I90">
+        <v>10</v>
+      </c>
+      <c r="J90">
+        <v>10</v>
+      </c>
+      <c r="K90">
+        <v>10</v>
+      </c>
+      <c r="L90">
+        <v>0.3</v>
+      </c>
+      <c r="M90">
+        <v>0.52503674487907726</v>
+      </c>
+      <c r="N90">
+        <v>2.5861223598861209</v>
+      </c>
+      <c r="O90">
+        <v>2.2436533690007789</v>
+      </c>
+      <c r="P90">
+        <v>0.28170915260861978</v>
+      </c>
+      <c r="Q90">
+        <v>0.28855209889159389</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>36</v>
+      </c>
+      <c r="B91">
+        <v>25</v>
+      </c>
+      <c r="C91" t="s">
+        <v>23</v>
+      </c>
+      <c r="D91">
+        <v>64.951176488518058</v>
+      </c>
+      <c r="E91">
+        <v>46.764847071733008</v>
+      </c>
+      <c r="F91">
+        <v>32.454803867782701</v>
+      </c>
+      <c r="G91">
+        <v>123.8052394865758</v>
+      </c>
+      <c r="H91">
+        <v>48.557073877163504</v>
+      </c>
+      <c r="I91">
+        <v>10</v>
+      </c>
+      <c r="J91">
+        <v>10</v>
+      </c>
+      <c r="K91">
+        <v>10</v>
+      </c>
+      <c r="L91">
+        <v>0.3</v>
+      </c>
+      <c r="M91">
+        <v>0.52469520802025205</v>
+      </c>
+      <c r="N91">
+        <v>2.6537211900112259</v>
+      </c>
+      <c r="O91">
+        <v>2.3094269897715658</v>
+      </c>
+      <c r="P91">
+        <v>0.27926609253007251</v>
+      </c>
+      <c r="Q91">
+        <v>0.2882750444652884</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>36</v>
+      </c>
+      <c r="B92">
+        <v>24</v>
+      </c>
+      <c r="C92" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92">
+        <v>63.09574947427754</v>
+      </c>
+      <c r="E92">
+        <v>45.428939621479827</v>
+      </c>
+      <c r="F92">
+        <v>31.527684097306999</v>
+      </c>
+      <c r="G92">
+        <v>123.4044008824736</v>
+      </c>
+      <c r="H92">
+        <v>48.444896484733839</v>
+      </c>
+      <c r="I92">
+        <v>10</v>
+      </c>
+      <c r="J92">
+        <v>10</v>
+      </c>
+      <c r="K92">
+        <v>10</v>
+      </c>
+      <c r="L92">
+        <v>0.3</v>
+      </c>
+      <c r="M92">
+        <v>0.52436463979736492</v>
+      </c>
+      <c r="N92">
+        <v>2.7236271666329261</v>
+      </c>
+      <c r="O92">
+        <v>2.377339222527993</v>
+      </c>
+      <c r="P92">
+        <v>0.2765567146696013</v>
+      </c>
+      <c r="Q92">
+        <v>0.28776016521720282</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>36</v>
+      </c>
+      <c r="B93">
+        <v>25</v>
+      </c>
+      <c r="C93" t="s">
+        <v>25</v>
+      </c>
+      <c r="D93">
+        <v>64.951176488518058</v>
+      </c>
+      <c r="E93">
+        <v>46.764847071733008</v>
+      </c>
+      <c r="F93">
+        <v>32.454803867782701</v>
+      </c>
+      <c r="G93">
+        <v>123.8052394865758</v>
+      </c>
+      <c r="H93">
+        <v>48.557073877163504</v>
+      </c>
+      <c r="I93">
+        <v>10</v>
+      </c>
+      <c r="J93">
+        <v>10</v>
+      </c>
+      <c r="K93">
+        <v>10</v>
+      </c>
+      <c r="L93">
+        <v>0.3</v>
+      </c>
+      <c r="M93">
+        <v>0.52469520802025205</v>
+      </c>
+      <c r="N93">
+        <v>2.6537211900112259</v>
+      </c>
+      <c r="O93">
+        <v>2.3094269897715658</v>
+      </c>
+      <c r="P93">
+        <v>0.27926609253007251</v>
+      </c>
+      <c r="Q93">
+        <v>0.2882750444652884</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>36</v>
+      </c>
+      <c r="B94">
+        <v>25</v>
+      </c>
+      <c r="C94" t="s">
+        <v>26</v>
+      </c>
+      <c r="D94">
+        <v>64.951176488518058</v>
+      </c>
+      <c r="E94">
+        <v>46.764847071733008</v>
+      </c>
+      <c r="F94">
+        <v>32.454803867782701</v>
+      </c>
+      <c r="G94">
+        <v>123.8052394865758</v>
+      </c>
+      <c r="H94">
+        <v>48.557073877163504</v>
+      </c>
+      <c r="I94">
+        <v>10</v>
+      </c>
+      <c r="J94">
+        <v>10</v>
+      </c>
+      <c r="K94">
+        <v>10</v>
+      </c>
+      <c r="L94">
+        <v>0.3</v>
+      </c>
+      <c r="M94">
+        <v>0.52469520802025205</v>
+      </c>
+      <c r="N94">
+        <v>2.6537211900112259</v>
+      </c>
+      <c r="O94">
+        <v>2.3094269897715658</v>
+      </c>
+      <c r="P94">
+        <v>0.27926609253007251</v>
+      </c>
+      <c r="Q94">
+        <v>0.2882750444652884</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>36</v>
+      </c>
+      <c r="B95">
+        <v>26</v>
+      </c>
+      <c r="C95" t="s">
+        <v>27</v>
+      </c>
+      <c r="D95">
+        <v>66.85524692559936</v>
+      </c>
+      <c r="E95">
+        <v>48.135777786431532</v>
+      </c>
+      <c r="F95">
+        <v>33.406229783783488</v>
+      </c>
+      <c r="G95">
+        <v>124.2218269962178</v>
+      </c>
+      <c r="H95">
+        <v>48.674021953782614</v>
+      </c>
+      <c r="I95">
+        <v>10</v>
+      </c>
+      <c r="J95">
+        <v>10</v>
+      </c>
+      <c r="K95">
+        <v>10</v>
+      </c>
+      <c r="L95">
+        <v>0.3</v>
+      </c>
+      <c r="M95">
+        <v>0.52503674487907726</v>
+      </c>
+      <c r="N95">
+        <v>2.5861223598861209</v>
+      </c>
+      <c r="O95">
+        <v>2.2436533690007789</v>
+      </c>
+      <c r="P95">
+        <v>0.28170915260861978</v>
+      </c>
+      <c r="Q95">
+        <v>0.28855209889159389</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>36</v>
+      </c>
+      <c r="B96">
+        <v>27</v>
+      </c>
+      <c r="C96" t="s">
+        <v>28</v>
+      </c>
+      <c r="D96">
+        <v>68.810668934896995</v>
+      </c>
+      <c r="E96">
+        <v>49.543681633125843</v>
+      </c>
+      <c r="F96">
+        <v>34.383315053389317</v>
+      </c>
+      <c r="G96">
+        <v>124.6551546843061</v>
+      </c>
+      <c r="H96">
+        <v>48.796056063123153</v>
+      </c>
+      <c r="I96">
+        <v>10</v>
+      </c>
+      <c r="J96">
+        <v>10</v>
+      </c>
+      <c r="K96">
+        <v>10</v>
+      </c>
+      <c r="L96">
+        <v>0.3</v>
+      </c>
+      <c r="M96">
+        <v>0.52538985263161764</v>
+      </c>
+      <c r="N96">
+        <v>2.520702289808205</v>
+      </c>
+      <c r="O96">
+        <v>2.1798945181294149</v>
+      </c>
+      <c r="P96">
+        <v>0.28389704955765799</v>
+      </c>
+      <c r="Q96">
+        <v>0.2885991717729951</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>36</v>
+      </c>
+      <c r="B97">
+        <v>28</v>
+      </c>
+      <c r="C97" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97">
+        <v>70.820362129811755</v>
+      </c>
+      <c r="E97">
+        <v>50.990660733464459</v>
+      </c>
+      <c r="F97">
+        <v>35.387518549024328</v>
+      </c>
+      <c r="G97">
+        <v>125.10629968854499</v>
+      </c>
+      <c r="H97">
+        <v>48.923519696935983</v>
+      </c>
+      <c r="I97">
+        <v>10</v>
+      </c>
+      <c r="J97">
+        <v>10</v>
+      </c>
+      <c r="K97">
+        <v>10</v>
+      </c>
+      <c r="L97">
+        <v>0.3</v>
+      </c>
+      <c r="M97">
+        <v>0.5257551807881673</v>
+      </c>
+      <c r="N97">
+        <v>2.457341563242633</v>
+      </c>
+      <c r="O97">
+        <v>2.118034919463617</v>
+      </c>
+      <c r="P97">
+        <v>0.2858400807349698</v>
+      </c>
+      <c r="Q97">
+        <v>0.28842336896168908</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>37</v>
+      </c>
+      <c r="B98">
+        <v>29</v>
+      </c>
+      <c r="C98" t="s">
+        <v>18</v>
+      </c>
+      <c r="D98">
+        <v>68.600377469091143</v>
+      </c>
+      <c r="E98">
+        <v>49.39227177774562</v>
+      </c>
+      <c r="F98">
+        <v>34.278236613755453</v>
+      </c>
+      <c r="G98">
+        <v>51.49348747471619</v>
+      </c>
+      <c r="H98">
+        <v>114.9692756176764</v>
+      </c>
+      <c r="I98">
+        <v>10</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0.7</v>
+      </c>
+      <c r="M98">
+        <v>0.51221277579244628</v>
+      </c>
+      <c r="N98">
+        <v>2.4265575385120099</v>
+      </c>
+      <c r="O98">
+        <v>2.1865768897202442</v>
+      </c>
+      <c r="P98">
+        <v>0.37983539926137577</v>
+      </c>
+      <c r="Q98">
+        <v>0.30485137057243039</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>37</v>
+      </c>
+      <c r="B99">
+        <v>30</v>
+      </c>
+      <c r="C99" t="s">
+        <v>19</v>
+      </c>
+      <c r="D99">
+        <v>70.429277000012462</v>
+      </c>
+      <c r="E99">
+        <v>50.709079440008971</v>
+      </c>
+      <c r="F99">
+        <v>35.192101131366222</v>
+      </c>
+      <c r="G99">
+        <v>51.597491415446719</v>
+      </c>
+      <c r="H99">
+        <v>115.1538830217799</v>
+      </c>
+      <c r="I99">
+        <v>10</v>
+      </c>
+      <c r="J99">
+        <v>0</v>
+      </c>
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0.7</v>
+      </c>
+      <c r="M99">
+        <v>0.51234941282186297</v>
+      </c>
+      <c r="N99">
+        <v>2.3676428545077508</v>
+      </c>
+      <c r="O99">
+        <v>2.1297961073769569</v>
+      </c>
+      <c r="P99">
+        <v>0.37966115281636459</v>
+      </c>
+      <c r="Q99">
+        <v>0.30497232873938401</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>37</v>
+      </c>
+      <c r="B100">
+        <v>29</v>
+      </c>
+      <c r="C100" t="s">
+        <v>20</v>
+      </c>
+      <c r="D100">
+        <v>68.600377469091143</v>
+      </c>
+      <c r="E100">
+        <v>49.39227177774562</v>
+      </c>
+      <c r="F100">
+        <v>34.278236613755453</v>
+      </c>
+      <c r="G100">
+        <v>51.49348747471619</v>
+      </c>
+      <c r="H100">
+        <v>114.9692756176764</v>
+      </c>
+      <c r="I100">
+        <v>10</v>
+      </c>
+      <c r="J100">
+        <v>0</v>
+      </c>
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>0.7</v>
+      </c>
+      <c r="M100">
+        <v>0.51221277579244628</v>
+      </c>
+      <c r="N100">
+        <v>2.4265575385120099</v>
+      </c>
+      <c r="O100">
+        <v>2.1865768897202442</v>
+      </c>
+      <c r="P100">
+        <v>0.37983539926137577</v>
+      </c>
+      <c r="Q100">
+        <v>0.30485137057243039</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>37</v>
+      </c>
+      <c r="B101">
+        <v>28</v>
+      </c>
+      <c r="C101" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101">
+        <v>66.811847481823193</v>
+      </c>
+      <c r="E101">
+        <v>48.104530186912697</v>
+      </c>
+      <c r="F101">
+        <v>33.384543949717411</v>
+      </c>
+      <c r="G101">
+        <v>51.393528969164471</v>
+      </c>
+      <c r="H101">
+        <v>114.7924515321272</v>
+      </c>
+      <c r="I101">
+        <v>10</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>0.7</v>
+      </c>
+      <c r="M101">
+        <v>0.51208003184314532</v>
+      </c>
+      <c r="N101">
+        <v>2.48737292508644</v>
+      </c>
+      <c r="O101">
+        <v>2.2451107947704769</v>
+      </c>
+      <c r="P101">
+        <v>0.37984917037668531</v>
+      </c>
+      <c r="Q101">
+        <v>0.30453987569528163</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>37</v>
+      </c>
+      <c r="B102">
+        <v>26</v>
+      </c>
+      <c r="C102" t="s">
+        <v>22</v>
+      </c>
+      <c r="D102">
+        <v>63.348366096718742</v>
+      </c>
+      <c r="E102">
+        <v>45.610823589637498</v>
+      </c>
+      <c r="F102">
+        <v>31.653911571208418</v>
+      </c>
+      <c r="G102">
+        <v>51.204780808329083</v>
+      </c>
+      <c r="H102">
+        <v>114.4602083696124</v>
+      </c>
+      <c r="I102">
+        <v>10</v>
+      </c>
+      <c r="J102">
+        <v>0</v>
+      </c>
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0.7</v>
+      </c>
+      <c r="M102">
+        <v>0.51182548907600556</v>
+      </c>
+      <c r="N102">
+        <v>2.6151422583655628</v>
+      </c>
+      <c r="O102">
+        <v>2.3678590189837521</v>
+      </c>
+      <c r="P102">
+        <v>0.37937136855258691</v>
+      </c>
+      <c r="Q102">
+        <v>0.30331984937386047</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>37</v>
+      </c>
+      <c r="B103">
+        <v>25</v>
+      </c>
+      <c r="C103" t="s">
+        <v>23</v>
+      </c>
+      <c r="D103">
+        <v>61.669958336027697</v>
+      </c>
+      <c r="E103">
+        <v>44.402370001939943</v>
+      </c>
+      <c r="F103">
+        <v>30.815244781346319</v>
+      </c>
+      <c r="G103">
+        <v>51.115557077116272</v>
+      </c>
+      <c r="H103">
+        <v>114.30391948654891</v>
+      </c>
+      <c r="I103">
+        <v>10</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0.7</v>
+      </c>
+      <c r="M103">
+        <v>0.51170335416408663</v>
+      </c>
+      <c r="N103">
+        <v>2.682334819529574</v>
+      </c>
+      <c r="O103">
+        <v>2.432302599957648</v>
+      </c>
+      <c r="P103">
+        <v>0.37886654287223159</v>
+      </c>
+      <c r="Q103">
+        <v>0.30239696395916721</v>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>37</v>
+      </c>
+      <c r="B104">
+        <v>24</v>
+      </c>
+      <c r="C104" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104">
+        <v>60.0249860339446</v>
+      </c>
+      <c r="E104">
+        <v>43.217989944440113</v>
+      </c>
+      <c r="F104">
+        <v>29.99328502144143</v>
+      </c>
+      <c r="G104">
+        <v>51.029506521480997</v>
+      </c>
+      <c r="H104">
+        <v>114.1536656678807</v>
+      </c>
+      <c r="I104">
+        <v>10</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0.7</v>
+      </c>
+      <c r="M104">
+        <v>0.5115844379320178</v>
+      </c>
+      <c r="N104">
+        <v>2.7519068825097159</v>
+      </c>
+      <c r="O104">
+        <v>2.4989593486148221</v>
+      </c>
+      <c r="P104">
+        <v>0.3781746402492917</v>
+      </c>
+      <c r="Q104">
+        <v>0.30125473454089879</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>37</v>
+      </c>
+      <c r="B105">
+        <v>25</v>
+      </c>
+      <c r="C105" t="s">
+        <v>25</v>
+      </c>
+      <c r="D105">
+        <v>61.669958336027697</v>
+      </c>
+      <c r="E105">
+        <v>44.402370001939943</v>
+      </c>
+      <c r="F105">
+        <v>30.815244781346319</v>
+      </c>
+      <c r="G105">
+        <v>51.115557077116272</v>
+      </c>
+      <c r="H105">
+        <v>114.30391948654891</v>
+      </c>
+      <c r="I105">
+        <v>10</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>0.7</v>
+      </c>
+      <c r="M105">
+        <v>0.51170335416408663</v>
+      </c>
+      <c r="N105">
+        <v>2.682334819529574</v>
+      </c>
+      <c r="O105">
+        <v>2.432302599957648</v>
+      </c>
+      <c r="P105">
+        <v>0.37886654287223159</v>
+      </c>
+      <c r="Q105">
+        <v>0.30239696395916721</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>37</v>
+      </c>
+      <c r="B106">
+        <v>25</v>
+      </c>
+      <c r="C106" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106">
+        <v>61.669958336027697</v>
+      </c>
+      <c r="E106">
+        <v>44.402370001939943</v>
+      </c>
+      <c r="F106">
+        <v>30.815244781346319</v>
+      </c>
+      <c r="G106">
+        <v>51.115557077116272</v>
+      </c>
+      <c r="H106">
+        <v>114.30391948654891</v>
+      </c>
+      <c r="I106">
+        <v>10</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>0.7</v>
+      </c>
+      <c r="M106">
+        <v>0.51170335416408663</v>
+      </c>
+      <c r="N106">
+        <v>2.682334819529574</v>
+      </c>
+      <c r="O106">
+        <v>2.432302599957648</v>
+      </c>
+      <c r="P106">
+        <v>0.37886654287223159</v>
+      </c>
+      <c r="Q106">
+        <v>0.30239696395916721</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>37</v>
+      </c>
+      <c r="B107">
+        <v>26</v>
+      </c>
+      <c r="C107" t="s">
+        <v>27</v>
+      </c>
+      <c r="D107">
+        <v>63.348366096718742</v>
+      </c>
+      <c r="E107">
+        <v>45.610823589637498</v>
+      </c>
+      <c r="F107">
+        <v>31.653911571208418</v>
+      </c>
+      <c r="G107">
+        <v>51.204780808329083</v>
+      </c>
+      <c r="H107">
+        <v>114.4602083696124</v>
+      </c>
+      <c r="I107">
+        <v>10</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>0.7</v>
+      </c>
+      <c r="M107">
+        <v>0.51182548907600556</v>
+      </c>
+      <c r="N107">
+        <v>2.6151422583655628</v>
+      </c>
+      <c r="O107">
+        <v>2.3678590189837521</v>
+      </c>
+      <c r="P107">
+        <v>0.37937136855258691</v>
+      </c>
+      <c r="Q107">
+        <v>0.30331984937386047</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>37</v>
+      </c>
+      <c r="B108">
+        <v>27</v>
+      </c>
+      <c r="C108" t="s">
+        <v>28</v>
+      </c>
+      <c r="D108">
+        <v>65.061772531109398</v>
+      </c>
+      <c r="E108">
+        <v>46.844476222398761</v>
+      </c>
+      <c r="F108">
+        <v>32.510066498344742</v>
+      </c>
+      <c r="G108">
+        <v>51.297368850615882</v>
+      </c>
+      <c r="H108">
+        <v>114.6229138001658</v>
+      </c>
+      <c r="I108">
+        <v>10</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>0.7</v>
+      </c>
+      <c r="M108">
+        <v>0.51195099423341806</v>
+      </c>
+      <c r="N108">
+        <v>2.5501961627535841</v>
+      </c>
+      <c r="O108">
+        <v>2.305501282312548</v>
+      </c>
+      <c r="P108">
+        <v>0.37969661147474232</v>
+      </c>
+      <c r="Q108">
+        <v>0.30403164695297102</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>37</v>
+      </c>
+      <c r="B109">
+        <v>28</v>
+      </c>
+      <c r="C109" t="s">
+        <v>29</v>
+      </c>
+      <c r="D109">
+        <v>66.811847481823193</v>
+      </c>
+      <c r="E109">
+        <v>48.104530186912697</v>
+      </c>
+      <c r="F109">
+        <v>33.384543949717411</v>
+      </c>
+      <c r="G109">
+        <v>51.393528969164471</v>
+      </c>
+      <c r="H109">
+        <v>114.7924515321272</v>
+      </c>
+      <c r="I109">
+        <v>10</v>
+      </c>
+      <c r="J109">
+        <v>0</v>
+      </c>
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>0.7</v>
+      </c>
+      <c r="M109">
+        <v>0.51208003184314532</v>
+      </c>
+      <c r="N109">
+        <v>2.48737292508644</v>
+      </c>
+      <c r="O109">
+        <v>2.2451107947704769</v>
+      </c>
+      <c r="P109">
+        <v>0.37984917037668531</v>
+      </c>
+      <c r="Q109">
+        <v>0.30453987569528163</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:Q109" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>